<commit_message>
Resultado das instâncias da simulação.
</commit_message>
<xml_diff>
--- a/ComputeResult/Resultados_Marcia/Resumo_Centralidade.xlsx
+++ b/ComputeResult/Resultados_Marcia/Resumo_Centralidade.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+  <si>
+    <t xml:space="preserve">LCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antigo</t>
+  </si>
   <si>
     <t xml:space="preserve">AS</t>
   </si>
@@ -49,6 +55,9 @@
   </si>
   <si>
     <t xml:space="preserve">Busca Local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRASP</t>
   </si>
   <si>
     <t xml:space="preserve">Abilene</t>
@@ -203,6 +212,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -212,10 +225,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -252,57 +261,77 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:K10"/>
+  <dimension ref="B1:O13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
+      <selection pane="topLeft" activeCell="N15" activeCellId="0" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.96356275303644"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="9" min="7" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.52631578947368"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.1619433198381"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.60728744939271"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.1619433198381"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="1"/>
+    </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="4" t="s">
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>8</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C3" s="6" t="n">
         <v>11</v>
@@ -328,10 +357,19 @@
       <c r="K3" s="8" t="n">
         <v>7</v>
       </c>
+      <c r="M3" s="8" t="n">
+        <v>7</v>
+      </c>
+      <c r="N3" s="8" t="n">
+        <v>7</v>
+      </c>
+      <c r="O3" s="8" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" s="6" t="n">
         <v>22</v>
@@ -357,10 +395,19 @@
       <c r="K4" s="8" t="n">
         <v>12</v>
       </c>
+      <c r="M4" s="8" t="n">
+        <v>12</v>
+      </c>
+      <c r="N4" s="8" t="n">
+        <v>12</v>
+      </c>
+      <c r="O4" s="8" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C5" s="6" t="n">
         <v>41</v>
@@ -386,10 +433,19 @@
       <c r="K5" s="8" t="n">
         <v>16</v>
       </c>
+      <c r="M5" s="8" t="n">
+        <v>16</v>
+      </c>
+      <c r="N5" s="8" t="n">
+        <v>16</v>
+      </c>
+      <c r="O5" s="8" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C6" s="6" t="n">
         <v>44</v>
@@ -415,10 +471,19 @@
       <c r="K6" s="8" t="n">
         <v>6</v>
       </c>
+      <c r="M6" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="N6" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="O6" s="8" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C7" s="6" t="n">
         <v>52</v>
@@ -444,10 +509,19 @@
       <c r="K7" s="8" t="n">
         <v>23</v>
       </c>
+      <c r="M7" s="8" t="n">
+        <v>22</v>
+      </c>
+      <c r="N7" s="8" t="n">
+        <v>22</v>
+      </c>
+      <c r="O7" s="8" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C8" s="6" t="n">
         <v>63</v>
@@ -473,10 +547,19 @@
       <c r="K8" s="8" t="n">
         <v>20</v>
       </c>
+      <c r="M8" s="8" t="n">
+        <v>20</v>
+      </c>
+      <c r="N8" s="8" t="n">
+        <v>20</v>
+      </c>
+      <c r="O8" s="8" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C9" s="6" t="n">
         <v>70</v>
@@ -502,10 +585,19 @@
       <c r="K9" s="8" t="n">
         <v>29</v>
       </c>
+      <c r="M9" s="8" t="n">
+        <v>29</v>
+      </c>
+      <c r="N9" s="8" t="n">
+        <v>28</v>
+      </c>
+      <c r="O9" s="8" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C10" s="6" t="n">
         <v>115</v>
@@ -531,7 +623,32 @@
       <c r="K10" s="8" t="n">
         <v>21</v>
       </c>
-    </row>
+      <c r="M10" s="8" t="n">
+        <v>21</v>
+      </c>
+      <c r="N10" s="8" t="n">
+        <v>21</v>
+      </c>
+      <c r="O10" s="8" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>